<commit_message>
Add cache route for clearing starting list cache; refactor Excel header handling for improved accuracy and flexibility.
</commit_message>
<xml_diff>
--- a/data/raslistar_live.xlsx
+++ b/data/raslistar_live.xlsx
@@ -6,13 +6,14 @@
   <sheets>
     <sheet sheetId="1" name="raslistar" state="visible" r:id="rId4"/>
     <sheet sheetId="2" name="Webhooks" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="einkunnir" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="153">
   <si>
     <t>Nr.</t>
   </si>
@@ -276,6 +277,201 @@
   </si>
   <si>
     <t>{"classId":70674,"competitionId":1,"eventId":999,"published":1}</t>
+  </si>
+  <si>
+    <t>knapi_nafn</t>
+  </si>
+  <si>
+    <t>hross_nafn</t>
+  </si>
+  <si>
+    <t>hross_fulltnafn</t>
+  </si>
+  <si>
+    <t>faedingarnumer</t>
+  </si>
+  <si>
+    <t>keppandi_numer</t>
+  </si>
+  <si>
+    <t>vallarnumer</t>
+  </si>
+  <si>
+    <t>saeti</t>
+  </si>
+  <si>
+    <t>keppandi_medaleinkunn</t>
+  </si>
+  <si>
+    <t>keppandi_einkunn_5_ds</t>
+  </si>
+  <si>
+    <t>einkunnir_domara</t>
+  </si>
+  <si>
+    <t>2026-02-05T14:52:33.715Z</t>
+  </si>
+  <si>
+    <t>71234</t>
+  </si>
+  <si>
+    <t>103300</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Oddur Ólafsson</t>
+  </si>
+  <si>
+    <t>Seifur</t>
+  </si>
+  <si>
+    <t>Seifur frá Borgarlandi</t>
+  </si>
+  <si>
+    <t>IS2019137219</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"6","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":6,"gangtegund":"Hægt tölt","keppandi_numer":543189},{"athugasemd":"","einkunn":6,"gangtegund":"Brokk","keppandi_numer":543189},{"athugasemd":"","einkunn":6,"gangtegund":"Fet","keppandi_numer":543189},{"athugasemd":"","einkunn":6,"gangtegund":"Stökk","keppandi_numer":543189},{"athugasemd":"","einkunn":6,"gangtegund":"Greitt tölt","keppandi_numer":543189}]}]</t>
+  </si>
+  <si>
+    <t>Sumarnótt</t>
+  </si>
+  <si>
+    <t>Sumarnótt frá Stóra-Kambi</t>
+  </si>
+  <si>
+    <t>IS2018237328</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"5","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":5,"gangtegund":"Hægt tölt","keppandi_numer":543171},{"athugasemd":"","einkunn":5,"gangtegund":"Brokk","keppandi_numer":543171},{"athugasemd":"","einkunn":5,"gangtegund":"Fet","keppandi_numer":543171},{"athugasemd":"","einkunn":5,"gangtegund":"Stökk","keppandi_numer":543171},{"athugasemd":"","einkunn":5,"gangtegund":"Greitt tölt","keppandi_numer":543171}]}]</t>
+  </si>
+  <si>
+    <t>Bringa</t>
+  </si>
+  <si>
+    <t>Bringa frá Borgarlandi</t>
+  </si>
+  <si>
+    <t>IS2018237218</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"5","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":5,"gangtegund":"Hægt tölt","keppandi_numer":543170},{"athugasemd":"","einkunn":5,"gangtegund":"Brokk","keppandi_numer":543170},{"athugasemd":"","einkunn":5,"gangtegund":"Fet","keppandi_numer":543170},{"athugasemd":"","einkunn":5,"gangtegund":"Stökk","keppandi_numer":543170},{"athugasemd":"","einkunn":5,"gangtegund":"Greitt tölt","keppandi_numer":543170}]}]</t>
+  </si>
+  <si>
+    <t>Þeódís</t>
+  </si>
+  <si>
+    <t>Þeódís frá Borgarlandi</t>
+  </si>
+  <si>
+    <t>IS2019237216</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"5","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":5,"gangtegund":"Hægt tölt","keppandi_numer":543169},{"athugasemd":"","einkunn":5,"gangtegund":"Brokk","keppandi_numer":543169},{"athugasemd":"","einkunn":5,"gangtegund":"Fet","keppandi_numer":543169},{"athugasemd":"","einkunn":5,"gangtegund":"Stökk","keppandi_numer":543169},{"athugasemd":"","einkunn":5,"gangtegund":"Greitt tölt","keppandi_numer":543169}]}]</t>
+  </si>
+  <si>
+    <t>Sóli</t>
+  </si>
+  <si>
+    <t>Sóli frá Borgarlandi</t>
+  </si>
+  <si>
+    <t>IS2023137215</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"5","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":5,"gangtegund":"Hægt tölt","keppandi_numer":543188},{"athugasemd":"","einkunn":5,"gangtegund":"Brokk","keppandi_numer":543188},{"athugasemd":"","einkunn":5,"gangtegund":"Fet","keppandi_numer":543188},{"athugasemd":"","einkunn":5,"gangtegund":"Stökk","keppandi_numer":543188},{"athugasemd":"","einkunn":5,"gangtegund":"Greitt tölt","keppandi_numer":543188}]}]</t>
+  </si>
+  <si>
+    <t>Oddviti</t>
+  </si>
+  <si>
+    <t>Oddviti frá Borgarlandi</t>
+  </si>
+  <si>
+    <t>IS2013137216</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"5","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":5,"gangtegund":"Hægt tölt","keppandi_numer":543172},{"athugasemd":"","einkunn":5,"gangtegund":"Brokk","keppandi_numer":543172},{"athugasemd":"","einkunn":5,"gangtegund":"Fet","keppandi_numer":543172},{"athugasemd":"","einkunn":5,"gangtegund":"Stökk","keppandi_numer":543172},{"athugasemd":"","einkunn":5,"gangtegund":"Greitt tölt","keppandi_numer":543172}]}]</t>
+  </si>
+  <si>
+    <t>Freyr</t>
+  </si>
+  <si>
+    <t>Freyr frá Borgarlandi</t>
+  </si>
+  <si>
+    <t>IS2019137215</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"0","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":null,"gangtegund":"Hægt tölt","keppandi_numer":1},{"athugasemd":"","einkunn":null,"gangtegund":"Brokk","keppandi_numer":1},{"athugasemd":"","einkunn":null,"gangtegund":"Fet","keppandi_numer":1},{"athugasemd":"","einkunn":null,"gangtegund":"Stökk","keppandi_numer":1},{"athugasemd":"","einkunn":null,"gangtegund":"Greitt tölt","keppandi_numer":1}]}]</t>
+  </si>
+  <si>
+    <t>Bjarmi</t>
+  </si>
+  <si>
+    <t>Bjarmi frá Borgarlandi</t>
+  </si>
+  <si>
+    <t>IS2015137219</t>
+  </si>
+  <si>
+    <t>2026-02-05T15:01:21.372Z</t>
+  </si>
+  <si>
+    <t>102919</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"8","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":8,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543168},{"athugasemd":"","einkunn":8,"gangtegund":"Hægt tölt","keppandi_numer":543168},{"athugasemd":"","einkunn":8,"gangtegund":"Tölt með slakan taum","keppandi_numer":543168}]}]</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"7,8","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":6,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543172},{"athugasemd":"","einkunn":7,"gangtegund":"Hægt tölt","keppandi_numer":543172},{"athugasemd":"","einkunn":9,"gangtegund":"Tölt með slakan taum","keppandi_numer":543172}]}]</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"7","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":7,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543169},{"athugasemd":"","einkunn":7,"gangtegund":"Hægt tölt","keppandi_numer":543169},{"athugasemd":"","einkunn":7,"gangtegund":"Tölt með slakan taum","keppandi_numer":543169}]}]</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"7","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":7,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543188},{"athugasemd":"","einkunn":7,"gangtegund":"Hægt tölt","keppandi_numer":543188},{"athugasemd":"","einkunn":7,"gangtegund":"Tölt með slakan taum","keppandi_numer":543188}]}]</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"6","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":6,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543189},{"athugasemd":"","einkunn":6,"gangtegund":"Hægt tölt","keppandi_numer":543189},{"athugasemd":"","einkunn":6,"gangtegund":"Tölt með slakan taum","keppandi_numer":543189}]}]</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"5","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":5,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543170},{"athugasemd":"","einkunn":5,"gangtegund":"Hægt tölt","keppandi_numer":543170},{"athugasemd":"","einkunn":5,"gangtegund":"Tölt með slakan taum","keppandi_numer":543170}]}]</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"4","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":4,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543171},{"athugasemd":"","einkunn":4,"gangtegund":"Hægt tölt","keppandi_numer":543171},{"athugasemd":"","einkunn":4,"gangtegund":"Tölt með slakan taum","keppandi_numer":543171}]}]</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"3","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":3,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543190},{"athugasemd":"","einkunn":3,"gangtegund":"Hægt tölt","keppandi_numer":543190},{"athugasemd":"","einkunn":3,"gangtegund":"Tölt með slakan taum","keppandi_numer":543190}]}]</t>
+  </si>
+  <si>
+    <t>2026-02-05T15:04:56.938Z</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"8,8","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":8,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543172},{"athugasemd":"","einkunn":9,"gangtegund":"Hægt tölt","keppandi_numer":543172},{"athugasemd":"","einkunn":9,"gangtegund":"Tölt með slakan taum","keppandi_numer":543172}]}]</t>
+  </si>
+  <si>
+    <t>2026-02-05T15:17:03.094Z</t>
+  </si>
+  <si>
+    <t>2026-02-05T15:30:34.820Z</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"8,5","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":8,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543172},{"athugasemd":"","einkunn":8,"gangtegund":"Hægt tölt","keppandi_numer":543172},{"athugasemd":"","einkunn":9,"gangtegund":"Tölt með slakan taum","keppandi_numer":543172}]}]</t>
+  </si>
+  <si>
+    <t>2026-02-05T15:37:02.636Z</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"8,3","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":7,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543172},{"athugasemd":"","einkunn":8,"gangtegund":"Hægt tölt","keppandi_numer":543172},{"athugasemd":"","einkunn":9,"gangtegund":"Tölt með slakan taum","keppandi_numer":543172}]}]</t>
+  </si>
+  <si>
+    <t>2026-02-05T15:42:00.620Z</t>
+  </si>
+  <si>
+    <t>[{"domarar":"Oddur Ólafsson","domari_adaleinkunn":"8","domsaeti_saeti":"1","sundurlidun_einkunna":[{"athugasemd":"","einkunn":6,"gangtegund":"Tölt frjáls hraði","keppandi_numer":543172},{"athugasemd":"","einkunn":8,"gangtegund":"Hægt tölt","keppandi_numer":543172},{"athugasemd":"","einkunn":9,"gangtegund":"Tölt með slakan taum","keppandi_numer":543172}]}]</t>
   </si>
 </sst>
 </file>
@@ -720,7 +916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -766,8 +962,26 @@
       <c r="O2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" t="s">
+        <v>30</v>
+      </c>
+      <c r="U2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -813,8 +1027,26 @@
       <c r="O3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s">
+        <v>30</v>
+      </c>
+      <c r="T3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -860,8 +1092,26 @@
       <c r="O4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P4">
+        <v>3</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -907,8 +1157,26 @@
       <c r="O5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P5">
+        <v>5</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -954,8 +1222,26 @@
       <c r="O6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>6</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" t="s">
+        <v>30</v>
+      </c>
+      <c r="T6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1001,8 +1287,26 @@
       <c r="O7" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P7">
+        <v>7</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" t="s">
+        <v>30</v>
+      </c>
+      <c r="T7" t="s">
+        <v>30</v>
+      </c>
+      <c r="U7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1047,6 +1351,24 @@
       </c>
       <c r="O8" t="s">
         <v>77</v>
+      </c>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R8" t="s">
+        <v>30</v>
+      </c>
+      <c r="S8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T8" t="s">
+        <v>30</v>
+      </c>
+      <c r="U8">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1118,4 +1440,2523 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N57"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G2" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2">
+        <v>543189</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3">
+        <v>543171</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4">
+        <v>543170</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I5">
+        <v>543169</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" t="s">
+        <v>120</v>
+      </c>
+      <c r="H6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6">
+        <v>543188</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>5</v>
+      </c>
+      <c r="M6" t="s">
+        <v>30</v>
+      </c>
+      <c r="N6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7">
+        <v>543172</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s">
+        <v>129</v>
+      </c>
+      <c r="I8">
+        <v>543190</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" t="s">
+        <v>131</v>
+      </c>
+      <c r="G9" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" t="s">
+        <v>133</v>
+      </c>
+      <c r="I9">
+        <v>543168</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" t="s">
+        <v>30</v>
+      </c>
+      <c r="N9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10">
+        <v>543168</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>8</v>
+      </c>
+      <c r="M10" t="s">
+        <v>30</v>
+      </c>
+      <c r="N10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>135</v>
+      </c>
+      <c r="D11" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11" t="s">
+        <v>125</v>
+      </c>
+      <c r="I11">
+        <v>543172</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>7.8</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" t="s">
+        <v>117</v>
+      </c>
+      <c r="I12">
+        <v>543169</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>7</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>134</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>120</v>
+      </c>
+      <c r="H13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13">
+        <v>543188</v>
+      </c>
+      <c r="J13">
+        <v>6</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>7</v>
+      </c>
+      <c r="M13" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14">
+        <v>543189</v>
+      </c>
+      <c r="J14">
+        <v>5</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="L14">
+        <v>6</v>
+      </c>
+      <c r="M14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" t="s">
+        <v>112</v>
+      </c>
+      <c r="H15" t="s">
+        <v>113</v>
+      </c>
+      <c r="I15">
+        <v>543170</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>6</v>
+      </c>
+      <c r="L15">
+        <v>5</v>
+      </c>
+      <c r="M15" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>134</v>
+      </c>
+      <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
+        <v>135</v>
+      </c>
+      <c r="D16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" t="s">
+        <v>109</v>
+      </c>
+      <c r="I16">
+        <v>543171</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <v>4</v>
+      </c>
+      <c r="M16" t="s">
+        <v>30</v>
+      </c>
+      <c r="N16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>127</v>
+      </c>
+      <c r="G17" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" t="s">
+        <v>129</v>
+      </c>
+      <c r="I17">
+        <v>543190</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>8</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17" t="s">
+        <v>30</v>
+      </c>
+      <c r="N17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F18" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" t="s">
+        <v>124</v>
+      </c>
+      <c r="H18" t="s">
+        <v>125</v>
+      </c>
+      <c r="I18">
+        <v>543172</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>8.8</v>
+      </c>
+      <c r="M18" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" t="s">
+        <v>133</v>
+      </c>
+      <c r="I19">
+        <v>543168</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19">
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <v>8</v>
+      </c>
+      <c r="M19" t="s">
+        <v>30</v>
+      </c>
+      <c r="N19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
+        <v>101</v>
+      </c>
+      <c r="E20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" t="s">
+        <v>120</v>
+      </c>
+      <c r="H20" t="s">
+        <v>121</v>
+      </c>
+      <c r="I20">
+        <v>543188</v>
+      </c>
+      <c r="J20">
+        <v>6</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20">
+        <v>7</v>
+      </c>
+      <c r="M20" t="s">
+        <v>30</v>
+      </c>
+      <c r="N20" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" t="s">
+        <v>115</v>
+      </c>
+      <c r="G21" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21">
+        <v>543169</v>
+      </c>
+      <c r="J21">
+        <v>7</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <v>7</v>
+      </c>
+      <c r="M21" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22">
+        <v>543189</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <v>6</v>
+      </c>
+      <c r="M22" t="s">
+        <v>30</v>
+      </c>
+      <c r="N22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>144</v>
+      </c>
+      <c r="B23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+      <c r="D23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" t="s">
+        <v>112</v>
+      </c>
+      <c r="H23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I23">
+        <v>543170</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>6</v>
+      </c>
+      <c r="L23">
+        <v>5</v>
+      </c>
+      <c r="M23" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" t="s">
+        <v>109</v>
+      </c>
+      <c r="I24">
+        <v>543171</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>7</v>
+      </c>
+      <c r="L24">
+        <v>4</v>
+      </c>
+      <c r="M24" t="s">
+        <v>30</v>
+      </c>
+      <c r="N24" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" t="s">
+        <v>135</v>
+      </c>
+      <c r="D25" t="s">
+        <v>101</v>
+      </c>
+      <c r="E25" t="s">
+        <v>102</v>
+      </c>
+      <c r="F25" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25">
+        <v>543190</v>
+      </c>
+      <c r="J25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>8</v>
+      </c>
+      <c r="L25">
+        <v>3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>30</v>
+      </c>
+      <c r="N25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
+        <v>135</v>
+      </c>
+      <c r="D26" t="s">
+        <v>101</v>
+      </c>
+      <c r="E26" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" t="s">
+        <v>124</v>
+      </c>
+      <c r="H26" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26">
+        <v>543172</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>8.8</v>
+      </c>
+      <c r="M26" t="s">
+        <v>30</v>
+      </c>
+      <c r="N26" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" t="s">
+        <v>133</v>
+      </c>
+      <c r="I27">
+        <v>543168</v>
+      </c>
+      <c r="J27">
+        <v>8</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27">
+        <v>8</v>
+      </c>
+      <c r="M27" t="s">
+        <v>30</v>
+      </c>
+      <c r="N27" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" t="s">
+        <v>119</v>
+      </c>
+      <c r="G28" t="s">
+        <v>120</v>
+      </c>
+      <c r="H28" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28">
+        <v>543188</v>
+      </c>
+      <c r="J28">
+        <v>6</v>
+      </c>
+      <c r="K28">
+        <v>3</v>
+      </c>
+      <c r="L28">
+        <v>7</v>
+      </c>
+      <c r="M28" t="s">
+        <v>30</v>
+      </c>
+      <c r="N28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" t="s">
+        <v>115</v>
+      </c>
+      <c r="G29" t="s">
+        <v>116</v>
+      </c>
+      <c r="H29" t="s">
+        <v>117</v>
+      </c>
+      <c r="I29">
+        <v>543169</v>
+      </c>
+      <c r="J29">
+        <v>7</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+      <c r="L29">
+        <v>7</v>
+      </c>
+      <c r="M29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H30" t="s">
+        <v>105</v>
+      </c>
+      <c r="I30">
+        <v>543189</v>
+      </c>
+      <c r="J30">
+        <v>5</v>
+      </c>
+      <c r="K30">
+        <v>5</v>
+      </c>
+      <c r="L30">
+        <v>6</v>
+      </c>
+      <c r="M30" t="s">
+        <v>30</v>
+      </c>
+      <c r="N30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" t="s">
+        <v>112</v>
+      </c>
+      <c r="H31" t="s">
+        <v>113</v>
+      </c>
+      <c r="I31">
+        <v>543170</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31">
+        <v>6</v>
+      </c>
+      <c r="L31">
+        <v>5</v>
+      </c>
+      <c r="M31" t="s">
+        <v>30</v>
+      </c>
+      <c r="N31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>135</v>
+      </c>
+      <c r="D32" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" t="s">
+        <v>107</v>
+      </c>
+      <c r="G32" t="s">
+        <v>108</v>
+      </c>
+      <c r="H32" t="s">
+        <v>109</v>
+      </c>
+      <c r="I32">
+        <v>543171</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <v>7</v>
+      </c>
+      <c r="L32">
+        <v>4</v>
+      </c>
+      <c r="M32" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="s">
+        <v>135</v>
+      </c>
+      <c r="D33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" t="s">
+        <v>127</v>
+      </c>
+      <c r="G33" t="s">
+        <v>128</v>
+      </c>
+      <c r="H33" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33">
+        <v>543190</v>
+      </c>
+      <c r="J33">
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <v>8</v>
+      </c>
+      <c r="L33">
+        <v>3</v>
+      </c>
+      <c r="M33" t="s">
+        <v>30</v>
+      </c>
+      <c r="N33" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" t="s">
+        <v>125</v>
+      </c>
+      <c r="I34">
+        <v>543172</v>
+      </c>
+      <c r="J34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>8.5</v>
+      </c>
+      <c r="M34" t="s">
+        <v>30</v>
+      </c>
+      <c r="N34" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" t="s">
+        <v>131</v>
+      </c>
+      <c r="G35" t="s">
+        <v>132</v>
+      </c>
+      <c r="H35" t="s">
+        <v>133</v>
+      </c>
+      <c r="I35">
+        <v>543168</v>
+      </c>
+      <c r="J35">
+        <v>8</v>
+      </c>
+      <c r="K35">
+        <v>2</v>
+      </c>
+      <c r="L35">
+        <v>8</v>
+      </c>
+      <c r="M35" t="s">
+        <v>30</v>
+      </c>
+      <c r="N35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36" t="s">
+        <v>119</v>
+      </c>
+      <c r="G36" t="s">
+        <v>120</v>
+      </c>
+      <c r="H36" t="s">
+        <v>121</v>
+      </c>
+      <c r="I36">
+        <v>543188</v>
+      </c>
+      <c r="J36">
+        <v>6</v>
+      </c>
+      <c r="K36">
+        <v>3</v>
+      </c>
+      <c r="L36">
+        <v>7</v>
+      </c>
+      <c r="M36" t="s">
+        <v>30</v>
+      </c>
+      <c r="N36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" t="s">
+        <v>101</v>
+      </c>
+      <c r="E37" t="s">
+        <v>102</v>
+      </c>
+      <c r="F37" t="s">
+        <v>115</v>
+      </c>
+      <c r="G37" t="s">
+        <v>116</v>
+      </c>
+      <c r="H37" t="s">
+        <v>117</v>
+      </c>
+      <c r="I37">
+        <v>543169</v>
+      </c>
+      <c r="J37">
+        <v>7</v>
+      </c>
+      <c r="K37">
+        <v>3</v>
+      </c>
+      <c r="L37">
+        <v>7</v>
+      </c>
+      <c r="M37" t="s">
+        <v>30</v>
+      </c>
+      <c r="N37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" t="s">
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D38" t="s">
+        <v>101</v>
+      </c>
+      <c r="E38" t="s">
+        <v>102</v>
+      </c>
+      <c r="F38" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" t="s">
+        <v>104</v>
+      </c>
+      <c r="H38" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38">
+        <v>543189</v>
+      </c>
+      <c r="J38">
+        <v>5</v>
+      </c>
+      <c r="K38">
+        <v>5</v>
+      </c>
+      <c r="L38">
+        <v>6</v>
+      </c>
+      <c r="M38" t="s">
+        <v>30</v>
+      </c>
+      <c r="N38" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" t="s">
+        <v>111</v>
+      </c>
+      <c r="G39" t="s">
+        <v>112</v>
+      </c>
+      <c r="H39" t="s">
+        <v>113</v>
+      </c>
+      <c r="I39">
+        <v>543170</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+      <c r="K39">
+        <v>6</v>
+      </c>
+      <c r="L39">
+        <v>5</v>
+      </c>
+      <c r="M39" t="s">
+        <v>30</v>
+      </c>
+      <c r="N39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" t="s">
+        <v>101</v>
+      </c>
+      <c r="E40" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" t="s">
+        <v>108</v>
+      </c>
+      <c r="H40" t="s">
+        <v>109</v>
+      </c>
+      <c r="I40">
+        <v>543171</v>
+      </c>
+      <c r="J40">
+        <v>2</v>
+      </c>
+      <c r="K40">
+        <v>7</v>
+      </c>
+      <c r="L40">
+        <v>4</v>
+      </c>
+      <c r="M40" t="s">
+        <v>30</v>
+      </c>
+      <c r="N40" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
+        <v>135</v>
+      </c>
+      <c r="D41" t="s">
+        <v>101</v>
+      </c>
+      <c r="E41" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" t="s">
+        <v>127</v>
+      </c>
+      <c r="G41" t="s">
+        <v>128</v>
+      </c>
+      <c r="H41" t="s">
+        <v>129</v>
+      </c>
+      <c r="I41">
+        <v>543190</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41">
+        <v>8</v>
+      </c>
+      <c r="L41">
+        <v>3</v>
+      </c>
+      <c r="M41" t="s">
+        <v>30</v>
+      </c>
+      <c r="N41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C42" t="s">
+        <v>135</v>
+      </c>
+      <c r="D42" t="s">
+        <v>101</v>
+      </c>
+      <c r="E42" t="s">
+        <v>102</v>
+      </c>
+      <c r="F42" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42" t="s">
+        <v>124</v>
+      </c>
+      <c r="H42" t="s">
+        <v>125</v>
+      </c>
+      <c r="I42">
+        <v>543172</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>8.3</v>
+      </c>
+      <c r="M42" t="s">
+        <v>30</v>
+      </c>
+      <c r="N42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" t="s">
+        <v>132</v>
+      </c>
+      <c r="H43" t="s">
+        <v>133</v>
+      </c>
+      <c r="I43">
+        <v>543168</v>
+      </c>
+      <c r="J43">
+        <v>8</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <v>8</v>
+      </c>
+      <c r="M43" t="s">
+        <v>30</v>
+      </c>
+      <c r="N43" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>149</v>
+      </c>
+      <c r="B44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" t="s">
+        <v>115</v>
+      </c>
+      <c r="G44" t="s">
+        <v>116</v>
+      </c>
+      <c r="H44" t="s">
+        <v>117</v>
+      </c>
+      <c r="I44">
+        <v>543169</v>
+      </c>
+      <c r="J44">
+        <v>7</v>
+      </c>
+      <c r="K44">
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <v>7</v>
+      </c>
+      <c r="M44" t="s">
+        <v>30</v>
+      </c>
+      <c r="N44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" t="s">
+        <v>135</v>
+      </c>
+      <c r="D45" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" t="s">
+        <v>119</v>
+      </c>
+      <c r="G45" t="s">
+        <v>120</v>
+      </c>
+      <c r="H45" t="s">
+        <v>121</v>
+      </c>
+      <c r="I45">
+        <v>543188</v>
+      </c>
+      <c r="J45">
+        <v>6</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>7</v>
+      </c>
+      <c r="M45" t="s">
+        <v>30</v>
+      </c>
+      <c r="N45" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>149</v>
+      </c>
+      <c r="B46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" t="s">
+        <v>101</v>
+      </c>
+      <c r="E46" t="s">
+        <v>102</v>
+      </c>
+      <c r="F46" t="s">
+        <v>103</v>
+      </c>
+      <c r="G46" t="s">
+        <v>104</v>
+      </c>
+      <c r="H46" t="s">
+        <v>105</v>
+      </c>
+      <c r="I46">
+        <v>543189</v>
+      </c>
+      <c r="J46">
+        <v>5</v>
+      </c>
+      <c r="K46">
+        <v>5</v>
+      </c>
+      <c r="L46">
+        <v>6</v>
+      </c>
+      <c r="M46" t="s">
+        <v>30</v>
+      </c>
+      <c r="N46" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" t="s">
+        <v>135</v>
+      </c>
+      <c r="D47" t="s">
+        <v>101</v>
+      </c>
+      <c r="E47" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" t="s">
+        <v>112</v>
+      </c>
+      <c r="H47" t="s">
+        <v>113</v>
+      </c>
+      <c r="I47">
+        <v>543170</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+      <c r="K47">
+        <v>6</v>
+      </c>
+      <c r="L47">
+        <v>5</v>
+      </c>
+      <c r="M47" t="s">
+        <v>30</v>
+      </c>
+      <c r="N47" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" t="s">
+        <v>135</v>
+      </c>
+      <c r="D48" t="s">
+        <v>101</v>
+      </c>
+      <c r="E48" t="s">
+        <v>102</v>
+      </c>
+      <c r="F48" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" t="s">
+        <v>108</v>
+      </c>
+      <c r="H48" t="s">
+        <v>109</v>
+      </c>
+      <c r="I48">
+        <v>543171</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>7</v>
+      </c>
+      <c r="L48">
+        <v>4</v>
+      </c>
+      <c r="M48" t="s">
+        <v>30</v>
+      </c>
+      <c r="N48" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>149</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+      <c r="C49" t="s">
+        <v>135</v>
+      </c>
+      <c r="D49" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" t="s">
+        <v>102</v>
+      </c>
+      <c r="F49" t="s">
+        <v>127</v>
+      </c>
+      <c r="G49" t="s">
+        <v>128</v>
+      </c>
+      <c r="H49" t="s">
+        <v>129</v>
+      </c>
+      <c r="I49">
+        <v>543190</v>
+      </c>
+      <c r="J49">
+        <v>3</v>
+      </c>
+      <c r="K49">
+        <v>8</v>
+      </c>
+      <c r="L49">
+        <v>3</v>
+      </c>
+      <c r="M49" t="s">
+        <v>30</v>
+      </c>
+      <c r="N49" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>135</v>
+      </c>
+      <c r="D50" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" t="s">
+        <v>102</v>
+      </c>
+      <c r="F50" t="s">
+        <v>131</v>
+      </c>
+      <c r="G50" t="s">
+        <v>132</v>
+      </c>
+      <c r="H50" t="s">
+        <v>133</v>
+      </c>
+      <c r="I50">
+        <v>543168</v>
+      </c>
+      <c r="J50">
+        <v>8</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>8</v>
+      </c>
+      <c r="M50" t="s">
+        <v>30</v>
+      </c>
+      <c r="N50" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" t="s">
+        <v>135</v>
+      </c>
+      <c r="D51" t="s">
+        <v>101</v>
+      </c>
+      <c r="E51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51" t="s">
+        <v>123</v>
+      </c>
+      <c r="G51" t="s">
+        <v>124</v>
+      </c>
+      <c r="H51" t="s">
+        <v>125</v>
+      </c>
+      <c r="I51">
+        <v>543172</v>
+      </c>
+      <c r="J51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>8</v>
+      </c>
+      <c r="M51" t="s">
+        <v>30</v>
+      </c>
+      <c r="N51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>151</v>
+      </c>
+      <c r="B52" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" t="s">
+        <v>135</v>
+      </c>
+      <c r="D52" t="s">
+        <v>101</v>
+      </c>
+      <c r="E52" t="s">
+        <v>102</v>
+      </c>
+      <c r="F52" t="s">
+        <v>119</v>
+      </c>
+      <c r="G52" t="s">
+        <v>120</v>
+      </c>
+      <c r="H52" t="s">
+        <v>121</v>
+      </c>
+      <c r="I52">
+        <v>543188</v>
+      </c>
+      <c r="J52">
+        <v>6</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <v>7</v>
+      </c>
+      <c r="M52" t="s">
+        <v>30</v>
+      </c>
+      <c r="N52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>151</v>
+      </c>
+      <c r="B53" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" t="s">
+        <v>101</v>
+      </c>
+      <c r="E53" t="s">
+        <v>102</v>
+      </c>
+      <c r="F53" t="s">
+        <v>115</v>
+      </c>
+      <c r="G53" t="s">
+        <v>116</v>
+      </c>
+      <c r="H53" t="s">
+        <v>117</v>
+      </c>
+      <c r="I53">
+        <v>543169</v>
+      </c>
+      <c r="J53">
+        <v>7</v>
+      </c>
+      <c r="K53">
+        <v>3</v>
+      </c>
+      <c r="L53">
+        <v>7</v>
+      </c>
+      <c r="M53" t="s">
+        <v>30</v>
+      </c>
+      <c r="N53" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>151</v>
+      </c>
+      <c r="B54" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" t="s">
+        <v>135</v>
+      </c>
+      <c r="D54" t="s">
+        <v>101</v>
+      </c>
+      <c r="E54" t="s">
+        <v>102</v>
+      </c>
+      <c r="F54" t="s">
+        <v>103</v>
+      </c>
+      <c r="G54" t="s">
+        <v>104</v>
+      </c>
+      <c r="H54" t="s">
+        <v>105</v>
+      </c>
+      <c r="I54">
+        <v>543189</v>
+      </c>
+      <c r="J54">
+        <v>5</v>
+      </c>
+      <c r="K54">
+        <v>5</v>
+      </c>
+      <c r="L54">
+        <v>6</v>
+      </c>
+      <c r="M54" t="s">
+        <v>30</v>
+      </c>
+      <c r="N54" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" t="s">
+        <v>101</v>
+      </c>
+      <c r="E55" t="s">
+        <v>102</v>
+      </c>
+      <c r="F55" t="s">
+        <v>111</v>
+      </c>
+      <c r="G55" t="s">
+        <v>112</v>
+      </c>
+      <c r="H55" t="s">
+        <v>113</v>
+      </c>
+      <c r="I55">
+        <v>543170</v>
+      </c>
+      <c r="J55">
+        <v>4</v>
+      </c>
+      <c r="K55">
+        <v>6</v>
+      </c>
+      <c r="L55">
+        <v>5</v>
+      </c>
+      <c r="M55" t="s">
+        <v>30</v>
+      </c>
+      <c r="N55" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" t="s">
+        <v>101</v>
+      </c>
+      <c r="E56" t="s">
+        <v>102</v>
+      </c>
+      <c r="F56" t="s">
+        <v>107</v>
+      </c>
+      <c r="G56" t="s">
+        <v>108</v>
+      </c>
+      <c r="H56" t="s">
+        <v>109</v>
+      </c>
+      <c r="I56">
+        <v>543171</v>
+      </c>
+      <c r="J56">
+        <v>2</v>
+      </c>
+      <c r="K56">
+        <v>7</v>
+      </c>
+      <c r="L56">
+        <v>4</v>
+      </c>
+      <c r="M56" t="s">
+        <v>30</v>
+      </c>
+      <c r="N56" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
+        <v>135</v>
+      </c>
+      <c r="D57" t="s">
+        <v>101</v>
+      </c>
+      <c r="E57" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" t="s">
+        <v>127</v>
+      </c>
+      <c r="G57" t="s">
+        <v>128</v>
+      </c>
+      <c r="H57" t="s">
+        <v>129</v>
+      </c>
+      <c r="I57">
+        <v>543190</v>
+      </c>
+      <c r="J57">
+        <v>3</v>
+      </c>
+      <c r="K57">
+        <v>8</v>
+      </c>
+      <c r="L57">
+        <v>3</v>
+      </c>
+      <c r="M57" t="s">
+        <v>30</v>
+      </c>
+      <c r="N57" t="s">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add ngrok autostart functionality in server.js; update webhooks.js to include writeDataSheet import; update binary Excel file.
</commit_message>
<xml_diff>
--- a/data/raslistar_live.xlsx
+++ b/data/raslistar_live.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>timestamp</t>
   </si>
@@ -44,6 +44,21 @@
     <t>{"classId":103060,"eventId":70617,"competitionId":3,"published":1}</t>
   </si>
   <si>
+    <t>2026-02-06T16:13:51.313Z</t>
+  </si>
+  <si>
+    <t>event_keppendalisti_breyta</t>
+  </si>
+  <si>
+    <t>71174</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>{"eventId":"71174"}</t>
+  </si>
+  <si>
     <t>Nr.</t>
   </si>
   <si>
@@ -99,9 +114,6 @@
   </si>
   <si>
     <t>E6</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>V</t>
@@ -582,103 +594,102 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="M1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="N1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="O1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="P1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="Q1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="R1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="S1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="J3">
         <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L3" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -686,40 +697,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
         <v>39</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I4" t="s">
-        <v>35</v>
       </c>
       <c r="J4">
         <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="M4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -727,40 +738,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" t="s">
         <v>39</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
       </c>
       <c r="J5">
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -768,40 +779,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="J6">
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L6" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -809,51 +820,51 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="I7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="J7">
         <v>7</v>
       </c>
       <c r="K7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L7" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="M7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
@@ -910,6 +921,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update .gitignore to exclude dist files; modify CLASS_ID in batch script; enhance app.cjs with ngrok autostart feature and new writeDataSheet function for Excel handling.
</commit_message>
<xml_diff>
--- a/data/raslistar_live.xlsx
+++ b/data/raslistar_live.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="2" name="Webhooks" state="visible" r:id="rId4"/>
+    <sheet sheetId="3" name="Webhooks" state="visible" r:id="rId4"/>
     <sheet sheetId="1" name="B-úrslit" state="visible" r:id="rId5"/>
+    <sheet sheetId="2" name="keppendalisti" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="188">
   <si>
     <t>timestamp</t>
   </si>
@@ -59,6 +60,9 @@
     <t>{"eventId":"71174"}</t>
   </si>
   <si>
+    <t>2026-02-06T16:19:56.727Z</t>
+  </si>
+  <si>
     <t>Nr.</t>
   </si>
   <si>
@@ -198,6 +202,381 @@
   </si>
   <si>
     <t>HELGA UNA BJÖRNSDÓTTIR</t>
+  </si>
+  <si>
+    <t>keppandi_numer</t>
+  </si>
+  <si>
+    <t>knapi_nafn</t>
+  </si>
+  <si>
+    <t>hross_nafn</t>
+  </si>
+  <si>
+    <t>hross_fulltnafn</t>
+  </si>
+  <si>
+    <t>faedingarnumer</t>
+  </si>
+  <si>
+    <t>knapi_adildarfelag</t>
+  </si>
+  <si>
+    <t>eigandi_adildarfelag</t>
+  </si>
+  <si>
+    <t>litur</t>
+  </si>
+  <si>
+    <t>varaknapi_nafn</t>
+  </si>
+  <si>
+    <t>varapar</t>
+  </si>
+  <si>
+    <t>keppnisgreinar</t>
+  </si>
+  <si>
+    <t>2026-02-06T16:19:56.841Z</t>
+  </si>
+  <si>
+    <t>Anna Sigríður Erlendsdóttir</t>
+  </si>
+  <si>
+    <t>Hlynur</t>
+  </si>
+  <si>
+    <t>Hlynur frá Árbæjarhjáleigu II</t>
+  </si>
+  <si>
+    <t>IS2018186756</t>
+  </si>
+  <si>
+    <t>Geysir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brúnn/dökk/sv. einlitt  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 1","hond":"H","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-unglingaflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Arney Brynja Sveinbjörnsdóttir</t>
+  </si>
+  <si>
+    <t>Gammur</t>
+  </si>
+  <si>
+    <t>Gammur frá Hvolsvelli</t>
+  </si>
+  <si>
+    <t>IS2003184977</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rauður/milli- stjörnótt  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Pollaflokkur","hond":"V","keppni":"1. sprettur","keppnisgrein":"Fimikeppni A","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Aron Dyröy Guðmundsson</t>
+  </si>
+  <si>
+    <t>Ísafold</t>
+  </si>
+  <si>
+    <t>Ísafold frá Kirkjubæ</t>
+  </si>
+  <si>
+    <t>IS2006286105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rauður/milli- blesótt  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 1","hond":"V","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-unglingaflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Arthúr Nói Guðmundsson</t>
+  </si>
+  <si>
+    <t>Húmfaxi</t>
+  </si>
+  <si>
+    <t>Húmfaxi frá Skálakoti</t>
+  </si>
+  <si>
+    <t>IS2016184160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grár/rauður einlitt  </t>
+  </si>
+  <si>
+    <t>Benedikt Leví Sveinbjörnsson</t>
+  </si>
+  <si>
+    <t>Eldur</t>
+  </si>
+  <si>
+    <t>Eldur frá Hvolsvelli</t>
+  </si>
+  <si>
+    <t>IS2017184978</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rauður/milli- einlitt  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 2","hond":"H","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-barnaflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Bjartey Stefnisdóttir</t>
+  </si>
+  <si>
+    <t>Kappi</t>
+  </si>
+  <si>
+    <t>Kappi frá Skíðbakka I</t>
+  </si>
+  <si>
+    <t>IS2005184367</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moldóttur/gul-/m- einlitt  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Pollaflokkur","hond":"H","keppni":"Forkeppni","keppnisgrein":"Pollatölt","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Dagur Stefnisson</t>
+  </si>
+  <si>
+    <t>Emilía</t>
+  </si>
+  <si>
+    <t>Emilía frá Feti</t>
+  </si>
+  <si>
+    <t>IS2008286918</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarpur/milli- einlitt  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 1","hond":"V","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-barnaflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Edda Sigurðardóttir</t>
+  </si>
+  <si>
+    <t>Brúða</t>
+  </si>
+  <si>
+    <t>Brúða frá Reykjavík</t>
+  </si>
+  <si>
+    <t>IS2018225484</t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 2","hond":"V","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-fullorðinsflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Eldey Yrsa Sveinbjörnsdóttir</t>
+  </si>
+  <si>
+    <t>Frosti</t>
+  </si>
+  <si>
+    <t>Frosti frá Hvolsvelli</t>
+  </si>
+  <si>
+    <t>IS2018184976</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brúnn/milli- einlitt  </t>
+  </si>
+  <si>
+    <t>Emilía Ösp Hjálmarsdóttir</t>
+  </si>
+  <si>
+    <t>Djörf</t>
+  </si>
+  <si>
+    <t>Djörf frá Búlandi</t>
+  </si>
+  <si>
+    <t>IS2016284320</t>
+  </si>
+  <si>
+    <t>Eva Hrönn Ásmundsdóttir</t>
+  </si>
+  <si>
+    <t>Theódór</t>
+  </si>
+  <si>
+    <t>Theódór frá Dalsholti</t>
+  </si>
+  <si>
+    <t>IS2005101185</t>
+  </si>
+  <si>
+    <t>Fríða Hansen</t>
+  </si>
+  <si>
+    <t>Vargur</t>
+  </si>
+  <si>
+    <t>Vargur frá Leirubakka</t>
+  </si>
+  <si>
+    <t>IS2012186704</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brúnn/milli- leistar(eingöngu)  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 1","hond":"H","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-fullorðinsflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Hulda Vaka Gísladóttir</t>
+  </si>
+  <si>
+    <t>Garún</t>
+  </si>
+  <si>
+    <t>Garún frá Brúnum</t>
+  </si>
+  <si>
+    <t>IS2009265299</t>
+  </si>
+  <si>
+    <t>Háfeti</t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 1","hond":"H","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-ungmennaflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Lina Sofie Peter</t>
+  </si>
+  <si>
+    <t>Aría</t>
+  </si>
+  <si>
+    <t>Aría frá Leirubakka</t>
+  </si>
+  <si>
+    <t>IS2019286705</t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 2","hond":"H","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-fullorðinsflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Lóa Dagmar Smáradóttir</t>
+  </si>
+  <si>
+    <t>Mandala</t>
+  </si>
+  <si>
+    <t>Mandala frá Breiðabólsstað</t>
+  </si>
+  <si>
+    <t>IS2019235726</t>
+  </si>
+  <si>
+    <t>Margrét Aþena Þorbjörnsdóttir</t>
+  </si>
+  <si>
+    <t>Fröken</t>
+  </si>
+  <si>
+    <t>Fröken frá Ásmúla</t>
+  </si>
+  <si>
+    <t>IS2019286303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Pollaflokkur","hond":"V","keppni":"Forkeppni","keppnisgrein":"Pollatölt","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Margrét Sóley Guðbergsdóttir</t>
+  </si>
+  <si>
+    <t>Læna</t>
+  </si>
+  <si>
+    <t>Læna frá Fitjarmýri</t>
+  </si>
+  <si>
+    <t>IS2019284140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarpur/milli- blesa auk leista eða sokka  </t>
+  </si>
+  <si>
+    <t>Orri Arnarson</t>
+  </si>
+  <si>
+    <t>Stallari</t>
+  </si>
+  <si>
+    <t>Stallari frá Leirubakka</t>
+  </si>
+  <si>
+    <t>IS2019186700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brúnn/mó- einlitt  </t>
+  </si>
+  <si>
+    <t>Pia Rumpf</t>
+  </si>
+  <si>
+    <t>Maístjarna</t>
+  </si>
+  <si>
+    <t>Maístjarna frá Arnarhóli</t>
+  </si>
+  <si>
+    <t>IS2019280582</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jarpur/milli- stjörnótt  </t>
+  </si>
+  <si>
+    <t>Salka Sigríður Sigurðardóttir</t>
+  </si>
+  <si>
+    <t>Bjarmi</t>
+  </si>
+  <si>
+    <t>Bjarmi frá Hrólfsstaðahelli</t>
+  </si>
+  <si>
+    <t>IS2018186801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grár/óþekktur einlitt  </t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 2","hond":"V","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-barnaflokkur","raslisti_birtur":0}]</t>
+  </si>
+  <si>
+    <t>Sigursteinn Ingi Jóhannsson</t>
+  </si>
+  <si>
+    <t>Hrynjandi</t>
+  </si>
+  <si>
+    <t>Hrynjandi frá Geysisholti</t>
+  </si>
+  <si>
+    <t>IS2018101499</t>
+  </si>
+  <si>
+    <t>[{"flokksteg":"Gæðingaflokkur 1","hond":"H","keppni":"Forkeppni","keppnisgrein":"Gæðingatölt-barnaflokkur","raslisti_birtur":0}]</t>
   </si>
 </sst>
 </file>
@@ -594,61 +973,61 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="P1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="R1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -662,34 +1041,34 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J3">
         <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L3" t="s">
         <v>13</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -703,34 +1082,34 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J4">
         <v>9</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L4" t="s">
         <v>13</v>
       </c>
       <c r="M4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -744,34 +1123,34 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J5">
         <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="L5" t="s">
         <v>13</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -785,34 +1164,34 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J6">
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L6" t="s">
         <v>13</v>
       </c>
       <c r="M6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -826,34 +1205,34 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="J7">
         <v>7</v>
       </c>
       <c r="K7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L7" t="s">
         <v>13</v>
       </c>
       <c r="M7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +1243,920 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:M22"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>543709</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>543830</v>
+      </c>
+      <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" t="s">
+        <v>79</v>
+      </c>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>543838</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I4" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>543889</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" t="s">
+        <v>98</v>
+      </c>
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>543829</v>
+      </c>
+      <c r="D6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>543629</v>
+      </c>
+      <c r="D7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>543630</v>
+      </c>
+      <c r="D8" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>543888</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" t="s">
+        <v>120</v>
+      </c>
+      <c r="H9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" t="s">
+        <v>79</v>
+      </c>
+      <c r="J9" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L9" t="s">
+        <v>13</v>
+      </c>
+      <c r="M9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>543831</v>
+      </c>
+      <c r="D10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" t="s">
+        <v>79</v>
+      </c>
+      <c r="I10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>543836</v>
+      </c>
+      <c r="D11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>130</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
+        <v>79</v>
+      </c>
+      <c r="J11" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" t="s">
+        <v>13</v>
+      </c>
+      <c r="M11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>543790</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J12" t="s">
+        <v>92</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>543934</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" t="s">
+        <v>138</v>
+      </c>
+      <c r="H13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I13" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" t="s">
+        <v>139</v>
+      </c>
+      <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>543840</v>
+      </c>
+      <c r="D14" t="s">
+        <v>141</v>
+      </c>
+      <c r="E14" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" t="s">
+        <v>143</v>
+      </c>
+      <c r="G14" t="s">
+        <v>144</v>
+      </c>
+      <c r="H14" t="s">
+        <v>145</v>
+      </c>
+      <c r="I14" t="s">
+        <v>145</v>
+      </c>
+      <c r="J14" t="s">
+        <v>126</v>
+      </c>
+      <c r="K14" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>543932</v>
+      </c>
+      <c r="D15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E15" t="s">
+        <v>148</v>
+      </c>
+      <c r="F15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" t="s">
+        <v>150</v>
+      </c>
+      <c r="H15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K15" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>543935</v>
+      </c>
+      <c r="D16" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" t="s">
+        <v>154</v>
+      </c>
+      <c r="G16" t="s">
+        <v>155</v>
+      </c>
+      <c r="H16" t="s">
+        <v>79</v>
+      </c>
+      <c r="I16" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" t="s">
+        <v>126</v>
+      </c>
+      <c r="K16" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>543771</v>
+      </c>
+      <c r="D17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G17" t="s">
+        <v>159</v>
+      </c>
+      <c r="H17" t="s">
+        <v>79</v>
+      </c>
+      <c r="I17" t="s">
+        <v>79</v>
+      </c>
+      <c r="J17" t="s">
+        <v>160</v>
+      </c>
+      <c r="K17" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>543832</v>
+      </c>
+      <c r="D18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E18" t="s">
+        <v>163</v>
+      </c>
+      <c r="F18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H18" t="s">
+        <v>79</v>
+      </c>
+      <c r="I18" t="s">
+        <v>79</v>
+      </c>
+      <c r="J18" t="s">
+        <v>166</v>
+      </c>
+      <c r="K18" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>543933</v>
+      </c>
+      <c r="D19" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F19" t="s">
+        <v>169</v>
+      </c>
+      <c r="G19" t="s">
+        <v>170</v>
+      </c>
+      <c r="H19" t="s">
+        <v>79</v>
+      </c>
+      <c r="I19" t="s">
+        <v>79</v>
+      </c>
+      <c r="J19" t="s">
+        <v>171</v>
+      </c>
+      <c r="K19" t="s">
+        <v>13</v>
+      </c>
+      <c r="L19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>543927</v>
+      </c>
+      <c r="D20" t="s">
+        <v>172</v>
+      </c>
+      <c r="E20" t="s">
+        <v>173</v>
+      </c>
+      <c r="F20" t="s">
+        <v>174</v>
+      </c>
+      <c r="G20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H20" t="s">
+        <v>79</v>
+      </c>
+      <c r="I20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" t="s">
+        <v>176</v>
+      </c>
+      <c r="K20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" t="s">
+        <v>13</v>
+      </c>
+      <c r="M20" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>543595</v>
+      </c>
+      <c r="D21" t="s">
+        <v>177</v>
+      </c>
+      <c r="E21" t="s">
+        <v>178</v>
+      </c>
+      <c r="F21" t="s">
+        <v>179</v>
+      </c>
+      <c r="G21" t="s">
+        <v>180</v>
+      </c>
+      <c r="H21" t="s">
+        <v>79</v>
+      </c>
+      <c r="I21" t="s">
+        <v>79</v>
+      </c>
+      <c r="J21" t="s">
+        <v>181</v>
+      </c>
+      <c r="K21" t="s">
+        <v>13</v>
+      </c>
+      <c r="L21" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>543936</v>
+      </c>
+      <c r="D22" t="s">
+        <v>183</v>
+      </c>
+      <c r="E22" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" t="s">
+        <v>185</v>
+      </c>
+      <c r="G22" t="s">
+        <v>186</v>
+      </c>
+      <c r="H22" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J22" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
@@ -944,6 +2236,29 @@
         <v>14</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Enhance Excel handling by introducing a new function to retrieve header information from a specified row, ensuring accurate data management. Rework the updateStartingListSheet function to recreate worksheets to prevent duplicate rows and streamline header processing. Update binary Excel file.
</commit_message>
<xml_diff>
--- a/data/raslistar_live.xlsx
+++ b/data/raslistar_live.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>timestamp</t>
   </si>
@@ -65,6 +65,63 @@
   </si>
   <si>
     <t>2026-02-06T21:15:33.795Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:01:21.562Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:02:08.841Z</t>
+  </si>
+  <si>
+    <t>{"classId":70674,"eventId":70674,"competitionId":1,"published":1}</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:02:52.439Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:03:53.610Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:12:32.161Z</t>
+  </si>
+  <si>
+    <t>{"classId":70674,"eventId":70674,"competitionId":2,"published":1}</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:12:36.440Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:14:06.748Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:14:26.229Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:14:36.775Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:16:11.742Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:16:27.774Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:19:12.265Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:19:23.415Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:19:57.101Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:20:09.228Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:20:30.863Z</t>
+  </si>
+  <si>
+    <t>2026-02-06T22:21:29.875Z</t>
   </si>
 </sst>
 </file>
@@ -441,7 +498,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G24"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
@@ -613,6 +670,397 @@
         <v>16</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>70617</v>
+      </c>
+      <c r="D8">
+        <v>103060</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>70674</v>
+      </c>
+      <c r="D9">
+        <v>70674</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>70674</v>
+      </c>
+      <c r="D10">
+        <v>70674</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>70674</v>
+      </c>
+      <c r="D11">
+        <v>70674</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>70674</v>
+      </c>
+      <c r="D12">
+        <v>70674</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>70674</v>
+      </c>
+      <c r="D13">
+        <v>70674</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>70674</v>
+      </c>
+      <c r="D14">
+        <v>70674</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>70674</v>
+      </c>
+      <c r="D15">
+        <v>70674</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>70674</v>
+      </c>
+      <c r="D16">
+        <v>70674</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>70674</v>
+      </c>
+      <c r="D17">
+        <v>70674</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>70674</v>
+      </c>
+      <c r="D18">
+        <v>70674</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>70674</v>
+      </c>
+      <c r="D19">
+        <v>70674</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>70674</v>
+      </c>
+      <c r="D20">
+        <v>70674</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>70674</v>
+      </c>
+      <c r="D21">
+        <v>70674</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>70674</v>
+      </c>
+      <c r="D22">
+        <v>70674</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>70674</v>
+      </c>
+      <c r="D23">
+        <v>70674</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>70674</v>
+      </c>
+      <c r="D24">
+        <v>70674</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>